<commit_message>
Ejercicios de excel y word en academia
</commit_message>
<xml_diff>
--- a/m1/Ejercicios/20191107/EjExcAva-Pra2.xlsx
+++ b/m1/Ejercicios/20191107/EjExcAva-Pra2.xlsx
@@ -216,7 +216,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="[$$-3C09]#,##0.00;\-[$$-3C09]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-3C09]#,##0.00;\-[$$-3C09]#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -305,8 +305,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -779,7 +779,14 @@
         <f ca="1">IF(YEARFRAC(C4,TODAY())&gt;40,IF(OR(D4="Cordon",D4="Centro"),150,200),100)</f>
         <v>150</v>
       </c>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="10">
+        <f ca="1">INT(YEARFRAC(C4,TODAY()))</f>
+        <v>63</v>
+      </c>
+      <c r="R4">
+        <f>IF(O4&lt;5000,300,IF(AND(O4&gt;=5000,O4&lt;=10000),IF(ISNUMBER(F4),200,100),0))</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -835,7 +842,14 @@
         <f t="shared" ref="P5:P32" ca="1" si="7">IF(YEARFRAC(C5,TODAY())&gt;40,IF(OR(D5="Cordon",D5="Centro"),150,200),100)</f>
         <v>200</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="10">
+        <f t="shared" ref="Q5:Q32" ca="1" si="8">INT(YEARFRAC(C5,TODAY()))</f>
+        <v>58</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R32" si="9">IF(O5&lt;5000,300,IF(AND(O5&gt;=5000,O5&lt;=10000),IF(ISNUMBER(F5),200,100),0))</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -891,7 +905,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -947,7 +968,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>54</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1003,7 +1031,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q8" s="10"/>
+      <c r="Q8" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -1059,7 +1094,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>100</v>
       </c>
-      <c r="Q9" s="10"/>
+      <c r="Q9" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1115,7 +1157,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q10" s="10"/>
+      <c r="Q10" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1171,7 +1220,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1227,7 +1283,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>150</v>
       </c>
-      <c r="Q12" s="10"/>
+      <c r="Q12" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1283,7 +1346,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q13" s="10"/>
+      <c r="Q13" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>49</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1339,7 +1409,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q14" s="10"/>
+      <c r="Q14" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>43</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1395,7 +1472,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q15" s="10"/>
+      <c r="Q15" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1451,9 +1535,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q16" s="10"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q16" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>52</v>
       </c>
@@ -1507,9 +1598,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q17" s="10"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q17" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>57</v>
       </c>
@@ -1563,9 +1661,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q18" s="10"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q18" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>59</v>
       </c>
@@ -1619,9 +1724,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q19" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>61</v>
       </c>
@@ -1675,9 +1787,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>42</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>69</v>
       </c>
@@ -1731,9 +1850,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q21" s="10"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q21" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>72</v>
       </c>
@@ -1787,9 +1913,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q22" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>46</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>78</v>
       </c>
@@ -1843,9 +1976,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>100</v>
       </c>
-      <c r="Q23" s="10"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>81</v>
       </c>
@@ -1899,9 +2039,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q24" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>84</v>
       </c>
@@ -1955,9 +2102,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>150</v>
       </c>
-      <c r="Q25" s="10"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q25" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>59</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>85</v>
       </c>
@@ -2011,9 +2165,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q26" s="10"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q26" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>86</v>
       </c>
@@ -2067,9 +2228,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>100</v>
       </c>
-      <c r="Q27" s="10"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q27" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>95</v>
       </c>
@@ -2123,9 +2291,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q28" s="10"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q28" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>43</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>98</v>
       </c>
@@ -2179,9 +2354,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q29" s="10"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q29" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>105</v>
       </c>
@@ -2235,9 +2417,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>150</v>
       </c>
-      <c r="Q30" s="10"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q30" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>44</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>113</v>
       </c>
@@ -2291,9 +2480,16 @@
         <f t="shared" ca="1" si="7"/>
         <v>100</v>
       </c>
-      <c r="Q31" s="10"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q31" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>123</v>
       </c>
@@ -2347,7 +2543,14 @@
         <f t="shared" ca="1" si="7"/>
         <v>200</v>
       </c>
-      <c r="Q32" s="10"/>
+      <c r="Q32" s="10">
+        <f t="shared" ca="1" si="8"/>
+        <v>74</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>

</xml_diff>